<commit_message>
Create Datagrid for forms
</commit_message>
<xml_diff>
--- a/Forms_Tutorial/input.xlsx
+++ b/Forms_Tutorial/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Uipath\Forms_Tutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F02C863-FE32-473A-ABFC-C3603DCE65A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED128EE4-1D68-4F33-B2C3-2D232A9227DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,16 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Fname</t>
-  </si>
-  <si>
-    <t>Sname</t>
-  </si>
-  <si>
-    <t>FullName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>a</t>
   </si>
@@ -48,10 +39,25 @@
     <t>f</t>
   </si>
   <si>
-    <t>a__1</t>
-  </si>
-  <si>
-    <t>S2 Fullname</t>
+    <t>field1</t>
+  </si>
+  <si>
+    <t>field2</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>field3</t>
   </si>
 </sst>
 </file>
@@ -372,20 +378,20 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -393,10 +399,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -404,10 +410,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -415,7 +421,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -423,7 +432,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>